<commit_message>
Major updates on result figures based on review #1
</commit_message>
<xml_diff>
--- a/Manuscript/Figures/4_Results/Fig_benchmark/Compare-scenarios.xlsx
+++ b/Manuscript/Figures/4_Results/Fig_benchmark/Compare-scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\GitHub\Downscaling-paper-manuscript\Manuscript\Figures\4_Results\Fig_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>Model</t>
   </si>
@@ -45,30 +45,18 @@
     <t>Directed Transition</t>
   </si>
   <si>
-    <t>AT127</t>
-  </si>
-  <si>
     <t>Centralized</t>
   </si>
   <si>
     <t>GWh/km**2</t>
   </si>
   <si>
-    <t>AT211</t>
-  </si>
-  <si>
     <t>AT221</t>
   </si>
   <si>
     <t>AT312</t>
   </si>
   <si>
-    <t>AT323</t>
-  </si>
-  <si>
-    <t>AT332</t>
-  </si>
-  <si>
     <t>AT342</t>
   </si>
   <si>
@@ -88,6 +76,9 @@
   </si>
   <si>
     <t>B_High</t>
+  </si>
+  <si>
+    <t>AT130</t>
   </si>
 </sst>
 </file>
@@ -427,16 +418,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -464,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -472,22 +463,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>1.5288320846308787</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -495,19 +486,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>4.0380912834999334</v>
+        <v>1.75</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -518,22 +509,22 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>1.2844795830469438</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -541,22 +532,22 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>3.5019580411417648</v>
+        <v>2.7</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -564,22 +555,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
-        <v>5.0873709556435172</v>
+        <v>2.13</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -587,22 +578,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0.90180307197940812</v>
+        <v>1.65</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -610,22 +601,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>1.9845157475480706</v>
+        <v>16.62</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -633,160 +624,22 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>1.7119754940640695</v>
+        <v>10.17</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>2.5135829837832437</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>1.1336855332014988</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>3.4212469788985671</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>1.3114770715068798</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>1.2766126261305031</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>3.0531479540499236</v>
-      </c>
-      <c r="G15" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>